<commit_message>
updated parsing for xlsx
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhisekjha/MyFolder/Github_Projects/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D06411-FEB3-4245-BB95-C7D7220984F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787B1D42-59FF-964D-8603-52FC14AC2F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{7EEE0C5F-63D3-364E-B1C2-A8E4E423EB72}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Serial No</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Completion Date</t>
   </si>
   <si>
-    <t>GitHub Link</t>
-  </si>
-  <si>
-    <t>Website Link</t>
-  </si>
-  <si>
     <t>https://github.com/abhisekjha/steganography</t>
   </si>
   <si>
@@ -99,6 +93,15 @@
   </si>
   <si>
     <t>https://www.abhisekjha.com.np/luxury-car-calculator</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Language Used</t>
   </si>
 </sst>
 </file>
@@ -482,22 +485,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931255D9-CD48-5947-9202-D1DCE34B8BCD}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
-    <col min="6" max="6" width="47.83203125" customWidth="1"/>
+    <col min="2" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" customWidth="1"/>
+    <col min="7" max="7" width="47.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,86 +508,94 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{D9DF53D2-BE31-9248-B00F-C3592D3A4C56}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{CAF64204-72E2-FC41-9F30-3D30D8E4DFBD}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{1683A4F5-3F3E-4F45-89A9-C02A24A1379C}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{E48480CF-A9BD-AF4F-8C92-D7F2A04D1FC9}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{26D4EC30-D4FB-7D47-9816-52D365AD4ECE}"/>
-    <hyperlink ref="F4" r:id="rId6" xr:uid="{DDD0E586-A4A4-F846-B4F0-8FFB16497AC6}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{D9DF53D2-BE31-9248-B00F-C3592D3A4C56}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{CAF64204-72E2-FC41-9F30-3D30D8E4DFBD}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{1683A4F5-3F3E-4F45-89A9-C02A24A1379C}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{E48480CF-A9BD-AF4F-8C92-D7F2A04D1FC9}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{26D4EC30-D4FB-7D47-9816-52D365AD4ECE}"/>
+    <hyperlink ref="G4" r:id="rId6" xr:uid="{DDD0E586-A4A4-F846-B4F0-8FFB16497AC6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added project in sheet
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhisekjha/MyFolder/Github_Projects/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787B1D42-59FF-964D-8603-52FC14AC2F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484B4F6E-4993-DE4C-9155-EB69D0D7A9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{7EEE0C5F-63D3-364E-B1C2-A8E4E423EB72}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Serial No</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>GitHub</t>
-  </si>
-  <si>
-    <t>Language Used</t>
   </si>
 </sst>
 </file>
@@ -485,22 +482,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931255D9-CD48-5947-9202-D1DCE34B8BCD}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="47.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+    <col min="6" max="6" width="47.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,94 +505,86 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
         <v>11</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
         <v>16</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{D9DF53D2-BE31-9248-B00F-C3592D3A4C56}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{CAF64204-72E2-FC41-9F30-3D30D8E4DFBD}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{1683A4F5-3F3E-4F45-89A9-C02A24A1379C}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{E48480CF-A9BD-AF4F-8C92-D7F2A04D1FC9}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{26D4EC30-D4FB-7D47-9816-52D365AD4ECE}"/>
-    <hyperlink ref="G4" r:id="rId6" xr:uid="{DDD0E586-A4A4-F846-B4F0-8FFB16497AC6}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D9DF53D2-BE31-9248-B00F-C3592D3A4C56}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{CAF64204-72E2-FC41-9F30-3D30D8E4DFBD}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{1683A4F5-3F3E-4F45-89A9-C02A24A1379C}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{E48480CF-A9BD-AF4F-8C92-D7F2A04D1FC9}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{26D4EC30-D4FB-7D47-9816-52D365AD4ECE}"/>
+    <hyperlink ref="F4" r:id="rId6" xr:uid="{DDD0E586-A4A4-F846-B4F0-8FFB16497AC6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated excel and gitignore
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhisekjha/MyFolder/Github_Projects/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF4341B-DD38-A54A-9FDD-4C6CCBE129D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA52D49-D865-C34B-8B75-CA4A4FE916A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{7EEE0C5F-63D3-364E-B1C2-A8E4E423EB72}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Serial No</t>
   </si>
@@ -134,10 +134,25 @@
     <t>Privacy Preserving Machine Learning</t>
   </si>
   <si>
-    <t>https://github.com/abhisekjha/privacy-preserving-ml</t>
-  </si>
-  <si>
     <t>https://www.abhisekjha.com.np/privacy-preserving-ml</t>
+  </si>
+  <si>
+    <t>https://github.com/abhisekjha/privacy-oreservc</t>
+  </si>
+  <si>
+    <t>https://github.com/abhisekjha/Chat-Bot</t>
+  </si>
+  <si>
+    <t>https://www.abhisekjha.com.np/Chat-Bot</t>
+  </si>
+  <si>
+    <t>6th May, 2024</t>
+  </si>
+  <si>
+    <t>8th May, 2024</t>
+  </si>
+  <si>
+    <t>Chat-bot Powered by GPT-4o</t>
   </si>
 </sst>
 </file>
@@ -182,10 +197,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -521,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931255D9-CD48-5947-9202-D1DCE34B8BCD}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,14 +676,40 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>33</v>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -682,8 +724,10 @@
     <hyperlink ref="F5" r:id="rId8" xr:uid="{02CD7884-FF9D-F740-8DA7-2A7FFE73CA91}"/>
     <hyperlink ref="E6" r:id="rId9" xr:uid="{97E7B1FC-DED7-8C43-AD3B-18C7C922CEAA}"/>
     <hyperlink ref="F6" r:id="rId10" xr:uid="{CAB151AB-0574-BF43-81F5-F3C7F5F4CF96}"/>
-    <hyperlink ref="B7" r:id="rId11" display="https://github.com/abhisekjha/privacy-preserving-ml" xr:uid="{A3D974DB-C9DA-C149-AE16-BFB517315A76}"/>
-    <hyperlink ref="F7" r:id="rId12" xr:uid="{EC394922-BEA6-B546-B583-ABD315F6B4FC}"/>
+    <hyperlink ref="F7" r:id="rId11" xr:uid="{EC394922-BEA6-B546-B583-ABD315F6B4FC}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{4F08F588-0400-5D4B-BBA3-5936A7F20B6B}"/>
+    <hyperlink ref="F8" r:id="rId13" xr:uid="{895867F6-53F5-B04F-8317-817F998503E3}"/>
+    <hyperlink ref="E8" r:id="rId14" xr:uid="{6E454319-EE7E-F245-B2FF-E0D3A75B8F4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>